<commit_message>
making a master preheim probe data sheet
</commit_message>
<xml_diff>
--- a/otu_data/WaterQualityData/PreheimProbeData/Compiled_EXO_Probe.xlsx
+++ b/otu_data/WaterQualityData/PreheimProbeData/Compiled_EXO_Probe.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/login/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/KeithSSD/CB_V4/otu_data/WaterQualityData/PreheimProbeData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAAADFD-0A9B-474B-A8C4-13AC02AEEF58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6EA1E4-F2F0-4744-B56D-492DE91ABEB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16100" xr2:uid="{175D3150-8069-BF48-BE7D-26D590479383}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="16100" xr2:uid="{175D3150-8069-BF48-BE7D-26D590479383}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,9 +98,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -146,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -156,12 +156,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,11 +476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B977BA-292A-DC48-87A7-16AD514AC292}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,15 +490,15 @@
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2970,7 +2970,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>42594</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>42594</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>42594</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>2.08</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>42594</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>2.44</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>42594</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -3243,43 +3243,40 @@
         <v>9078.5280000000002</v>
       </c>
       <c r="H55" s="12">
-        <v>8736.8510000000006</v>
+        <v>8769.6659999999993</v>
       </c>
       <c r="I55" s="12">
-        <v>8769.6659999999993</v>
+        <v>5700.2820000000002</v>
       </c>
       <c r="J55" s="12">
-        <v>5700.2820000000002</v>
+        <v>4.875</v>
       </c>
       <c r="K55" s="12">
-        <v>4.875</v>
+        <v>103.94799999999999</v>
       </c>
       <c r="L55" s="12">
-        <v>103.94799999999999</v>
+        <v>8.0830000000000002</v>
       </c>
       <c r="M55" s="12">
-        <v>8.0830000000000002</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="N55" s="12">
-        <v>0.40799999999999997</v>
+        <v>8.3569999999999993</v>
       </c>
       <c r="O55" s="12">
-        <v>8.3569999999999993</v>
+        <v>143.893</v>
       </c>
       <c r="P55" s="12">
-        <v>143.893</v>
+        <v>2.3820000000000001</v>
       </c>
       <c r="Q55" s="12">
-        <v>2.3820000000000001</v>
+        <v>38.997</v>
       </c>
       <c r="R55" s="12">
-        <v>76.358999999999995</v>
-      </c>
-      <c r="S55" s="12">
-        <v>38.997</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+        <v>-76.358999999999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C58" s="1"/>
     </row>
   </sheetData>

</xml_diff>